<commit_message>
Updated Stage 2 Now Assigned View Do not edit
</commit_message>
<xml_diff>
--- a/Planning/JAC Modpack.xlsx
+++ b/Planning/JAC Modpack.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c81d479feedaae75/JAC Pack Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joshua\SkyDrive\JAC Pack Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,10 +17,10 @@
     <sheet name="Timeline" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Main!$A$2:$F$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Main!$A$2:$M$36</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Ores!$A$2:$H$2</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="125">
   <si>
     <t>Item Breakdown</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Time-Craft</t>
-  </si>
-  <si>
     <t>Ore</t>
   </si>
   <si>
@@ -137,9 +134,6 @@
     <t>Flux-Capicitor</t>
   </si>
   <si>
-    <t>Glass</t>
-  </si>
-  <si>
     <t>Plutonium</t>
   </si>
   <si>
@@ -221,9 +215,6 @@
     <t>5, 51</t>
   </si>
   <si>
-    <t>5, 52</t>
-  </si>
-  <si>
     <t>1, 33</t>
   </si>
   <si>
@@ -275,9 +266,6 @@
     <t>Alexbegt</t>
   </si>
   <si>
-    <t>8 to 18</t>
-  </si>
-  <si>
     <t>Texture Artist Assigned</t>
   </si>
   <si>
@@ -291,13 +279,139 @@
   </si>
   <si>
     <t>Textures</t>
+  </si>
+  <si>
+    <t>Basic items and world generation</t>
+  </si>
+  <si>
+    <t>Getting machines and functions to make ores to ingots ect.</t>
+  </si>
+  <si>
+    <t>Static</t>
+  </si>
+  <si>
+    <t>Not Started</t>
+  </si>
+  <si>
+    <t>In Development</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>Status (Dev)</t>
+  </si>
+  <si>
+    <t>Status (Textures)</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Silver Ingot</t>
+  </si>
+  <si>
+    <t>Windshield</t>
+  </si>
+  <si>
+    <t>Time-Traveler</t>
+  </si>
+  <si>
+    <t>NEI Item ID</t>
+  </si>
+  <si>
+    <t>Damage Value</t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>Rickaba</t>
+  </si>
+  <si>
+    <t>Component of Pounder</t>
+  </si>
+  <si>
+    <t>2x2x1 TBD Design</t>
+  </si>
+  <si>
+    <t>Bottler</t>
+  </si>
+  <si>
+    <t>Pump</t>
+  </si>
+  <si>
+    <t>Tank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customizable </t>
+  </si>
+  <si>
+    <t>Compressor</t>
+  </si>
+  <si>
+    <t>Melter</t>
+  </si>
+  <si>
+    <t>Evaporator</t>
+  </si>
+  <si>
+    <t>If we can find some use for it</t>
+  </si>
+  <si>
+    <t>Tools</t>
+  </si>
+  <si>
+    <t>NubStuff</t>
+  </si>
+  <si>
+    <t>Armor</t>
+  </si>
+  <si>
+    <t>Hazmat Armor</t>
+  </si>
+  <si>
+    <t>Titanium Tools</t>
+  </si>
+  <si>
+    <t>Aluminum Tools</t>
+  </si>
+  <si>
+    <t>Copper Tools</t>
+  </si>
+  <si>
+    <t>Tin Tools</t>
+  </si>
+  <si>
+    <t>Silver Tools</t>
+  </si>
+  <si>
+    <t>Aluminum Armor</t>
+  </si>
+  <si>
+    <t>Copper Armor</t>
+  </si>
+  <si>
+    <t>Tin Armor</t>
+  </si>
+  <si>
+    <t>Silver Armor</t>
+  </si>
+  <si>
+    <t>Blocks</t>
+  </si>
+  <si>
+    <t>TBD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -342,17 +456,73 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="8"/>
-      <name val="Segoe UI"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -373,7 +543,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -393,8 +563,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -418,8 +596,40 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="19"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="19" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="19" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="20"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="20" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="22"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="22" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="21"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="21" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="23"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="23" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="24"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="24" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="25"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="25" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="26"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="26" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="22" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="21" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="24" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="20" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="27">
+    <cellStyle name="Accent1" xfId="21" builtinId="29"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33"/>
+    <cellStyle name="Accent3" xfId="23" builtinId="37"/>
+    <cellStyle name="Accent4" xfId="24" builtinId="41"/>
+    <cellStyle name="Accent5" xfId="25" builtinId="45"/>
+    <cellStyle name="Accent6" xfId="26" builtinId="49"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -429,6 +639,7 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Good" xfId="19" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -438,6 +649,7 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Neutral" xfId="20" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -454,7 +666,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -762,13 +974,13 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>876300</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>190501</xdr:rowOff>
+          <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -841,14 +1053,19 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>19050</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>828675</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3089" name="Check Box 17" hidden="1">
@@ -914,20 +1131,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>876300</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>76200</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3090" name="Check Box 18" hidden="1">
@@ -993,20 +1215,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>19050</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>828675</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3091" name="Check Box 19" hidden="1">
@@ -1072,20 +1299,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>876300</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>5</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
-        </xdr:from>
-        <xdr:ext cx="809625" cy="209550"/>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3092" name="Check Box 20" hidden="1">
@@ -1151,20 +1383,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>19050</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>828675</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3093" name="Check Box 21" hidden="1">
@@ -1230,20 +1467,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>876300</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>76200</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3094" name="Check Box 22" hidden="1">
@@ -1309,20 +1551,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>19050</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>828675</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3095" name="Check Box 23" hidden="1">
@@ -1388,20 +1635,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>866775</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>714375</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3096" name="Check Box 24" hidden="1">
@@ -1467,7 +1719,7 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -1799,26 +2051,30 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:M66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5" customWidth="1"/>
     <col min="2" max="2" width="12.125" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="22.875" customWidth="1"/>
-    <col min="6" max="6" width="39.375" style="6" customWidth="1"/>
-    <col min="8" max="8" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1826,7 +2082,7 @@
       <c r="C1" s="1"/>
       <c r="F1" s="5"/>
     </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1840,156 +2096,359 @@
         <v>3</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="H3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="K3" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="L3" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="M3" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="H4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="K4" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="L4" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="M4" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="H5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="K5" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="L5" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="M5" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
-      <c r="H6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="K6" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="L6" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="M6" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
-      <c r="H7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="K7" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="L7" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="M7" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
       <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="H8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="J8" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="K8" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="L8" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="M8" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
-      <c r="H9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="K9" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="L9" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="M9" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="15"/>
+      <c r="J10" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="K10" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="L10" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="M10" s="22" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>28000</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <f>G11+256</f>
+        <v>28256</v>
+      </c>
+      <c r="J11" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="K11" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="L11" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="M11" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>28000</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <f t="shared" ref="I12:I36" si="0">G12+256</f>
+        <v>28256</v>
+      </c>
+      <c r="J12" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="K12" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="L12" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="M12" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="H13" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <v>28000</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J13" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="K13" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="L13" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="M13" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
-      <c r="H14" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <v>28000</v>
+      </c>
+      <c r="H14">
+        <v>3</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J14" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="K14" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="L14" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="M14" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -1997,13 +2456,32 @@
       <c r="E15">
         <v>1</v>
       </c>
-      <c r="H15" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>28000</v>
+      </c>
+      <c r="H15">
+        <v>4</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J15" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="K15" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="L15" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="M15" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D16" t="s">
         <v>18</v>
@@ -2011,13 +2489,32 @@
       <c r="E16">
         <v>1</v>
       </c>
-      <c r="H16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>28000</v>
+      </c>
+      <c r="H16">
+        <v>5</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J16" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="K16" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="L16" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="M16" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D17" t="s">
         <v>19</v>
@@ -2025,41 +2522,98 @@
       <c r="E17">
         <v>1</v>
       </c>
-      <c r="H17" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>28000</v>
+      </c>
+      <c r="H17">
+        <v>6</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J17" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="K17" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="L17" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="M17" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D18" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="E18">
         <v>1</v>
       </c>
-      <c r="H18" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>28000</v>
+      </c>
+      <c r="H18">
+        <v>7</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J18" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="K18" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="L18" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="M18" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
-      <c r="H19" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>28000</v>
+      </c>
+      <c r="H19">
+        <v>8</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J19" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="K19" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="L19" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="M19" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D20" t="s">
         <v>45</v>
@@ -2067,354 +2621,1267 @@
       <c r="E20">
         <v>1</v>
       </c>
-      <c r="H20" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>28000</v>
+      </c>
+      <c r="H20">
+        <v>9</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J20" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="K20" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="L20" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="M20" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D21" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="E21">
         <v>1</v>
       </c>
-      <c r="H21" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>28000</v>
+      </c>
+      <c r="H21">
+        <v>10</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J21" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="K21" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="L21" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="M21" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D22" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E22">
         <v>1</v>
       </c>
-      <c r="H22" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <v>28000</v>
+      </c>
+      <c r="H22">
+        <v>11</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J22" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="K22" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="L22" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="M22" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D23" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E23">
         <v>1</v>
       </c>
-      <c r="H23" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" t="s">
-        <v>28</v>
-      </c>
-      <c r="E24">
+      <c r="G23">
+        <v>28000</v>
+      </c>
+      <c r="H23">
+        <v>12</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J23" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="K23" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="L23" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="M23" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="3:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="3">
         <v>1</v>
       </c>
-      <c r="H24" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="F24" s="15"/>
+      <c r="G24" s="3">
+        <v>28000</v>
+      </c>
+      <c r="H24" s="3">
+        <v>13</v>
+      </c>
+      <c r="I24" s="3">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J24" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="K24" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="L24" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="M24" s="22" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D25" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="E25">
-        <v>1</v>
-      </c>
-      <c r="H25" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="G25">
+        <v>28000</v>
+      </c>
+      <c r="H25">
+        <v>22</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J25" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="K25" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="L25" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="M25" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="G26">
+        <v>28000</v>
+      </c>
+      <c r="H26">
+        <v>23</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J26" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="K26" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="L26" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="M26" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D27" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E27">
         <v>2</v>
       </c>
-      <c r="H27" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
+      <c r="G27">
+        <v>28000</v>
+      </c>
+      <c r="H27">
+        <v>24</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J27" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="K27" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="L27" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="M27" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="3:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="3">
+        <v>2</v>
+      </c>
+      <c r="F28" s="15"/>
+      <c r="G28" s="3">
+        <v>28000</v>
+      </c>
+      <c r="H28" s="3">
+        <v>25</v>
+      </c>
+      <c r="I28" s="3">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J28" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="K28" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="L28" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="M28" s="22" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>28000</v>
+      </c>
+      <c r="H29">
         <v>14</v>
       </c>
-      <c r="D28" t="s">
-        <v>26</v>
-      </c>
-      <c r="E28">
-        <v>2</v>
-      </c>
-      <c r="H28" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29" t="s">
-        <v>27</v>
-      </c>
-      <c r="E29">
-        <v>2</v>
-      </c>
-      <c r="H29" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J29" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="K29" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="L29" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="M29" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="3:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="D30" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E30">
-        <v>2</v>
-      </c>
-      <c r="H30" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>28000</v>
+      </c>
+      <c r="H30">
+        <v>15</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J30" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="K30" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="L30" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="M30" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>28000</v>
+      </c>
+      <c r="H31">
+        <v>16</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J31" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="K31" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="L31" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="M31" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>30</v>
+        <v>94</v>
       </c>
       <c r="E32">
         <v>1</v>
       </c>
-      <c r="H32" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="33" spans="3:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G32">
+        <v>28000</v>
+      </c>
+      <c r="H32">
+        <v>17</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J32" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="K32" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="L32" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="M32" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D33" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E33">
         <v>1</v>
       </c>
-      <c r="H33" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G33">
+        <v>28000</v>
+      </c>
+      <c r="H33">
+        <v>18</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J33" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="K33" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="L33" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="M33" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D34" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E34">
         <v>1</v>
       </c>
-      <c r="H34" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="35" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G34">
+        <v>28000</v>
+      </c>
+      <c r="H34">
+        <v>19</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J34" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="K34" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="L34" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="M34" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D35" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E35">
         <v>1</v>
       </c>
-      <c r="H35" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>32</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="G35">
+        <v>28000</v>
+      </c>
+      <c r="H35">
+        <v>20</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J35" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="K35" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="L35" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="M35" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="36" spans="3:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C36" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E36" s="3">
+        <v>1</v>
+      </c>
+      <c r="F36" s="15"/>
+      <c r="G36" s="3">
+        <v>28000</v>
+      </c>
+      <c r="H36" s="3">
+        <v>21</v>
+      </c>
+      <c r="I36" s="3">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J36" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="K36" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="L36" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="M36" s="22" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
         <v>37</v>
       </c>
-      <c r="E36">
-        <v>1</v>
-      </c>
-      <c r="H36" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="37" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
-        <v>32</v>
-      </c>
       <c r="D37" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="E37">
-        <v>1</v>
-      </c>
-      <c r="H37" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="38" spans="3:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="J37" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="K37" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="L37" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="M37" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D38" t="s">
+        <v>102</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+      <c r="J38" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="K38" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="L38" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="M38" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="39" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39" t="s">
+        <v>103</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+      <c r="J39" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="K39" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="L39" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="M39" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>37</v>
+      </c>
+      <c r="D40" t="s">
+        <v>108</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="J40" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="K40" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="L40" s="21"/>
+      <c r="M40" s="21"/>
+    </row>
+    <row r="41" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>37</v>
+      </c>
+      <c r="D41" t="s">
+        <v>107</v>
+      </c>
+      <c r="E41">
+        <v>2</v>
+      </c>
+      <c r="J41" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="K41" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="L41" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="M41" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="3:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C42" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E42" s="3">
+        <v>2</v>
+      </c>
+      <c r="F42" s="15"/>
+      <c r="J42" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="K42" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="L42" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="M42" s="22" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>40</v>
+      </c>
+      <c r="D43" t="s">
         <v>38</v>
-      </c>
-      <c r="E38">
-        <v>1</v>
-      </c>
-      <c r="H38" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="39" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
-        <v>32</v>
-      </c>
-      <c r="D39" t="s">
-        <v>29</v>
-      </c>
-      <c r="E39">
-        <v>1</v>
-      </c>
-      <c r="H39" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="43" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
-        <v>39</v>
-      </c>
-      <c r="D43" t="s">
-        <v>46</v>
       </c>
       <c r="E43">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="F43" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J43" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="K43" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="L43" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="M43" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" spans="3:13" ht="26.25" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D44" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E44">
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="F44" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="J44" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="K44" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="L44" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="M44" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="D45" t="s">
+        <v>48</v>
       </c>
       <c r="E45">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="F45" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="J45" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="K45" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="L45" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="M45" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="D46" t="s">
+        <v>104</v>
       </c>
       <c r="E46">
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C47" t="s">
+      <c r="F46" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="J46" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="K46" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="L46" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="M46" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="3:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C47" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E47" s="3">
+        <v>2</v>
+      </c>
+      <c r="F47" s="15"/>
+      <c r="J47" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="K47" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="L47" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="M47" s="22" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C48" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="D48" t="s">
+        <v>114</v>
+      </c>
+      <c r="E48" s="16">
+        <v>2</v>
+      </c>
+      <c r="J48" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="K48" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="L48" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="M48" s="38" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="49" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C49" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="D49" t="s">
+        <v>115</v>
+      </c>
+      <c r="E49" s="16">
+        <v>2</v>
+      </c>
+      <c r="J49" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="K49" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="L49" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="M49" s="38" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="50" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C50" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="D50" t="s">
+        <v>116</v>
+      </c>
+      <c r="E50" s="16">
+        <v>2</v>
+      </c>
+      <c r="J50" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="K50" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="L50" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="M50" s="38" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="51" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C51" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="D51" t="s">
+        <v>117</v>
+      </c>
+      <c r="E51" s="16">
+        <v>2</v>
+      </c>
+      <c r="J51" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="K51" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="L51" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="M51" s="38" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="52" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C52" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="D52" t="s">
+        <v>118</v>
+      </c>
+      <c r="E52" s="16">
+        <v>2</v>
+      </c>
+      <c r="J52" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="K52" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="L52" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="M52" s="38" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="53" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C53" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="D53" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="16">
+        <v>2</v>
+      </c>
+      <c r="J53" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="K53" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="L53" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="M53" s="38" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="54" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C54" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="D54" t="s">
+        <v>119</v>
+      </c>
+      <c r="E54" s="16">
+        <v>2</v>
+      </c>
+      <c r="J54" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="K54" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="L54" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="M54" s="38" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="55" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C55" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="D55" t="s">
+        <v>120</v>
+      </c>
+      <c r="E55" s="16">
+        <v>2</v>
+      </c>
+      <c r="J55" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="K55" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="L55" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="M55" s="38" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="56" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C56" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="D56" t="s">
+        <v>121</v>
+      </c>
+      <c r="E56" s="16">
+        <v>2</v>
+      </c>
+      <c r="J56" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="K56" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="L56" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="M56" s="38" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="57" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C57" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="D57" t="s">
+        <v>122</v>
+      </c>
+      <c r="E57" s="16">
+        <v>2</v>
+      </c>
+      <c r="J57" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="K57" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="L57" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="M57" s="38" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="58" spans="3:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C58" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E58" s="3">
+        <v>2</v>
+      </c>
+      <c r="F58" s="15"/>
+      <c r="J58" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="K58" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="L58" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="M58" s="22" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="59" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C59" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="D59" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="16">
+        <v>2</v>
+      </c>
+      <c r="J59" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="K59" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="L59" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="M59" s="38" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="60" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C60" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="D60" t="s">
+        <v>9</v>
+      </c>
+      <c r="E60" s="16">
+        <v>2</v>
+      </c>
+      <c r="J60" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="K60" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="L60" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="M60" s="38" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="61" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C61" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="D61" t="s">
+        <v>10</v>
+      </c>
+      <c r="E61" s="16">
+        <v>2</v>
+      </c>
+      <c r="J61" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="K61" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="L61" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="M61" s="38" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="62" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C62" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="D62" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" s="16">
+        <v>2</v>
+      </c>
+      <c r="J62" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="K62" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="L62" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="M62" s="38" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="63" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C63" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="D63" t="s">
+        <v>12</v>
+      </c>
+      <c r="E63" s="16">
+        <v>2</v>
+      </c>
+      <c r="J63" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="K63" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="L63" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="M63" s="38" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="64" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C64" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="D64" t="s">
+        <v>98</v>
+      </c>
+      <c r="E64" s="16">
+        <v>2</v>
+      </c>
+      <c r="J64" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="K64" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="L64" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="M64" s="38" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="65" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C65" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="D65" t="s">
+        <v>23</v>
+      </c>
+      <c r="E65" s="16">
+        <v>2</v>
+      </c>
+      <c r="J65" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="K65" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="L65" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="M65" s="38" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="66" spans="3:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C66" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="D66" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E47">
+      <c r="E66" s="17">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C48" t="s">
-        <v>39</v>
-      </c>
-      <c r="E48">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C49" t="s">
-        <v>39</v>
-      </c>
-      <c r="E49">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
-        <v>39</v>
-      </c>
-      <c r="E50">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C54" t="s">
-        <v>42</v>
-      </c>
-      <c r="D54" t="s">
-        <v>40</v>
-      </c>
-      <c r="E54">
-        <v>2</v>
-      </c>
-      <c r="F54" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="H54" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="55" spans="3:8" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="C55" t="s">
-        <v>42</v>
-      </c>
-      <c r="D55" t="s">
-        <v>48</v>
-      </c>
-      <c r="E55">
-        <v>2</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H55" t="s">
-        <v>80</v>
+      <c r="F66" s="15"/>
+      <c r="J66" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="K66" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="L66" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="M66" s="22" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:F37"/>
+  <autoFilter ref="A2:M36"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -2434,13 +3901,13 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.25" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.125" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.625" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.375" style="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.875" style="10" bestFit="1" customWidth="1"/>
@@ -2453,7 +3920,7 @@
   <sheetData>
     <row r="1" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -2467,42 +3934,42 @@
         <v>3</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>7</v>
+        <v>95</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G3" s="10">
         <v>25</v>
@@ -2511,27 +3978,27 @@
         <v>102</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>7</v>
+        <v>95</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G4" s="10">
         <v>25</v>
@@ -2540,27 +4007,27 @@
         <v>102</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>7</v>
+        <v>95</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G5" s="10">
         <v>25</v>
@@ -2569,27 +4036,27 @@
         <v>102</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>7</v>
+        <v>95</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G6" s="10">
         <v>5</v>
@@ -2598,27 +4065,27 @@
         <v>20</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>7</v>
+        <v>95</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G7" s="10">
         <v>5</v>
@@ -2627,27 +4094,27 @@
         <v>20</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>7</v>
+        <v>95</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G8" s="10">
         <v>3</v>
@@ -2656,36 +4123,36 @@
         <v>7</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>57</v>
-      </c>
       <c r="E9" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="G9" s="10">
-        <v>13</v>
-      </c>
-      <c r="H9" s="10">
-        <v>170</v>
+        <v>92</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>92</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2705,10 +4172,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2717,35 +4184,39 @@
     <col min="2" max="2" width="5.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5" customWidth="1"/>
-    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>41342</v>
       </c>
@@ -2753,71 +4224,92 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="F3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>124</v>
+      </c>
       <c r="B4" s="13">
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="F4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>86</v>
+      </c>
       <c r="B5" s="13">
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>86</v>
+      </c>
       <c r="B6" s="13">
         <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>86</v>
+      </c>
       <c r="B7" s="13">
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>86</v>
+      </c>
       <c r="B8" s="13">
         <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="13"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="13"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="13"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="13"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="13"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="13"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="13"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" s="13"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
@@ -3021,16 +4513,16 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>876300</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>85725</xdr:colOff>
+                    <xdr:colOff>0</xdr:colOff>
                     <xdr:row>6</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3109,16 +4601,16 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>866775</xdr:colOff>
                     <xdr:row>7</xdr:row>
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>4</xdr:col>
-                    <xdr:colOff>85725</xdr:colOff>
-                    <xdr:row>8</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>714375</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>190500</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>

</xml_diff>

<commit_message>
Something i've been thinging about
I may be quitting, i just can't take this anymore.
</commit_message>
<xml_diff>
--- a/Planning/JAC Modpack.xlsx
+++ b/Planning/JAC Modpack.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c81d479feedaae75/JAC Pack Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexander\Documents\GitHub\jacpack\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="31515" windowHeight="20325" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="31515" windowHeight="20325" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -17,10 +17,10 @@
     <sheet name="Timeline" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Main!$A$2:$F$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Main!$A$2:$M$36</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Ores!$A$2:$H$2</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="123">
   <si>
     <t>Item Breakdown</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Time-Craft</t>
-  </si>
-  <si>
     <t>Ore</t>
   </si>
   <si>
@@ -137,9 +134,6 @@
     <t>Flux-Capicitor</t>
   </si>
   <si>
-    <t>Glass</t>
-  </si>
-  <si>
     <t>Plutonium</t>
   </si>
   <si>
@@ -221,9 +215,6 @@
     <t>5, 51</t>
   </si>
   <si>
-    <t>5, 52</t>
-  </si>
-  <si>
     <t>1, 33</t>
   </si>
   <si>
@@ -266,18 +257,9 @@
     <t>Zmaster</t>
   </si>
   <si>
-    <t>alexbegt</t>
-  </si>
-  <si>
     <t>xFinity</t>
   </si>
   <si>
-    <t>Alexbegt</t>
-  </si>
-  <si>
-    <t>8 to 18</t>
-  </si>
-  <si>
     <t>Texture Artist Assigned</t>
   </si>
   <si>
@@ -291,13 +273,139 @@
   </si>
   <si>
     <t>Textures</t>
+  </si>
+  <si>
+    <t>Basic items and world generation</t>
+  </si>
+  <si>
+    <t>Getting machines and functions to make ores to ingots ect.</t>
+  </si>
+  <si>
+    <t>Static</t>
+  </si>
+  <si>
+    <t>Not Started</t>
+  </si>
+  <si>
+    <t>In Development</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>Status (Dev)</t>
+  </si>
+  <si>
+    <t>Status (Textures)</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Silver Ingot</t>
+  </si>
+  <si>
+    <t>Windshield</t>
+  </si>
+  <si>
+    <t>Time-Traveler</t>
+  </si>
+  <si>
+    <t>NEI Item ID</t>
+  </si>
+  <si>
+    <t>Damage Value</t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>Rickaba</t>
+  </si>
+  <si>
+    <t>Component of Pounder</t>
+  </si>
+  <si>
+    <t>2x2x1 TBD Design</t>
+  </si>
+  <si>
+    <t>Bottler</t>
+  </si>
+  <si>
+    <t>Pump</t>
+  </si>
+  <si>
+    <t>Tank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customizable </t>
+  </si>
+  <si>
+    <t>Compressor</t>
+  </si>
+  <si>
+    <t>Melter</t>
+  </si>
+  <si>
+    <t>Evaporator</t>
+  </si>
+  <si>
+    <t>If we can find some use for it</t>
+  </si>
+  <si>
+    <t>Tools</t>
+  </si>
+  <si>
+    <t>NubStuff</t>
+  </si>
+  <si>
+    <t>Armor</t>
+  </si>
+  <si>
+    <t>Hazmat Armor</t>
+  </si>
+  <si>
+    <t>Titanium Tools</t>
+  </si>
+  <si>
+    <t>Aluminum Tools</t>
+  </si>
+  <si>
+    <t>Copper Tools</t>
+  </si>
+  <si>
+    <t>Tin Tools</t>
+  </si>
+  <si>
+    <t>Silver Tools</t>
+  </si>
+  <si>
+    <t>Aluminum Armor</t>
+  </si>
+  <si>
+    <t>Copper Armor</t>
+  </si>
+  <si>
+    <t>Tin Armor</t>
+  </si>
+  <si>
+    <t>Silver Armor</t>
+  </si>
+  <si>
+    <t>Blocks</t>
+  </si>
+  <si>
+    <t>TBD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -342,17 +450,68 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="8"/>
-      <name val="Segoe UI"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -373,7 +532,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -393,8 +552,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -418,8 +584,38 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="19"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="19" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="19" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="20"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="20" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="22"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="22" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="21"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="21" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="23"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="23" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="24"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="24" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="25"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="25" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="22" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="21" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="24" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="20" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="25" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="26">
+    <cellStyle name="Accent1" xfId="21" builtinId="29"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33"/>
+    <cellStyle name="Accent3" xfId="23" builtinId="37"/>
+    <cellStyle name="Accent4" xfId="24" builtinId="41"/>
+    <cellStyle name="Accent6" xfId="25" builtinId="49"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -429,6 +625,7 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Good" xfId="19" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -438,6 +635,7 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Neutral" xfId="20" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -454,7 +652,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -762,13 +960,13 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>876300</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>190501</xdr:rowOff>
+          <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -841,14 +1039,19 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>19050</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>828675</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3089" name="Check Box 17" hidden="1">
@@ -914,20 +1117,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>876300</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>76200</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3090" name="Check Box 18" hidden="1">
@@ -993,20 +1201,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>19050</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>828675</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3091" name="Check Box 19" hidden="1">
@@ -1072,20 +1285,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>876300</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>5</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
-        </xdr:from>
-        <xdr:ext cx="809625" cy="209550"/>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3092" name="Check Box 20" hidden="1">
@@ -1151,20 +1369,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>19050</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>828675</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3093" name="Check Box 21" hidden="1">
@@ -1230,20 +1453,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>876300</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>76200</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3094" name="Check Box 22" hidden="1">
@@ -1309,20 +1537,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>19050</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>828675</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3095" name="Check Box 23" hidden="1">
@@ -1388,20 +1621,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>866775</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>714375</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3096" name="Check Box 24" hidden="1">
@@ -1467,7 +1705,7 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -1799,26 +2037,30 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:M66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
+      <selection pane="bottomLeft" activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5" customWidth="1"/>
     <col min="2" max="2" width="12.125" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="22.875" customWidth="1"/>
-    <col min="6" max="6" width="39.375" style="6" customWidth="1"/>
-    <col min="8" max="8" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1826,7 +2068,7 @@
       <c r="C1" s="1"/>
       <c r="F1" s="5"/>
     </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1840,581 +2082,1808 @@
         <v>3</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H2" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="H3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="K3" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="L3" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="M3" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="H4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="K4" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="L4" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="M4" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="H5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="K5" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="L5" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="M5" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
-      <c r="H6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="K6" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="L6" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="M6" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
-      <c r="H7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="K7" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="L7" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="M7" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>96</v>
       </c>
       <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="H8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="J8" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="K8" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="L8" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="M8" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
-      <c r="H9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
+      <c r="J9" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="K9" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="L9" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="M9" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="J10" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K10" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="L10" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="M10" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="2">
+        <v>28000</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2">
+        <f>G11+256</f>
+        <v>28256</v>
+      </c>
+      <c r="J11" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K11" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="L11" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="M11" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E13">
+      <c r="E12" s="2">
         <v>1</v>
       </c>
-      <c r="H13" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
+      <c r="F12" s="5"/>
+      <c r="G12" s="2">
+        <v>28000</v>
+      </c>
+      <c r="H12" s="2">
+        <v>1</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" ref="I12:I36" si="0">G12+256</f>
+        <v>28256</v>
+      </c>
+      <c r="J12" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K12" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="L12" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="M12" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="2">
+        <v>28000</v>
+      </c>
+      <c r="H13" s="2">
+        <v>2</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J13" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K13" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="L13" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="M13" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="2">
+        <v>28000</v>
+      </c>
+      <c r="H14" s="2">
+        <v>3</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J14" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K14" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="L14" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="M14" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="2">
+        <v>28000</v>
+      </c>
+      <c r="H15" s="2">
+        <v>4</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J15" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K15" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="L15" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="M15" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="G16" s="2">
+        <v>28000</v>
+      </c>
+      <c r="H16" s="2">
+        <v>5</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J16" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K16" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="L16" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="M16" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="3:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="2">
+        <v>1</v>
+      </c>
+      <c r="F17" s="5"/>
+      <c r="G17" s="2">
+        <v>28000</v>
+      </c>
+      <c r="H17" s="2">
+        <v>6</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J17" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K17" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="L17" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="M17" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="2">
+        <v>1</v>
+      </c>
+      <c r="F18" s="5"/>
+      <c r="G18" s="2">
+        <v>28000</v>
+      </c>
+      <c r="H18" s="2">
+        <v>7</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J18" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K18" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="L18" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="M18" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1</v>
+      </c>
+      <c r="F19" s="5"/>
+      <c r="G19" s="2">
+        <v>28000</v>
+      </c>
+      <c r="H19" s="2">
+        <v>8</v>
+      </c>
+      <c r="I19" s="2">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J19" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K19" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="L19" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="M19" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="3:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1</v>
+      </c>
+      <c r="F20" s="5"/>
+      <c r="G20" s="2">
+        <v>28000</v>
+      </c>
+      <c r="H20" s="2">
+        <v>9</v>
+      </c>
+      <c r="I20" s="2">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J20" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K20" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="L20" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="M20" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="3:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="2">
+        <v>1</v>
+      </c>
+      <c r="F21" s="5"/>
+      <c r="G21" s="2">
+        <v>28000</v>
+      </c>
+      <c r="H21" s="2">
+        <v>10</v>
+      </c>
+      <c r="I21" s="2">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J21" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K21" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="L21" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="M21" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="3:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="2">
+        <v>1</v>
+      </c>
+      <c r="F22" s="5"/>
+      <c r="G22" s="2">
+        <v>28000</v>
+      </c>
+      <c r="H22" s="2">
+        <v>11</v>
+      </c>
+      <c r="I22" s="2">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J22" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K22" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="L22" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="M22" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1</v>
+      </c>
+      <c r="F23" s="5"/>
+      <c r="G23" s="2">
+        <v>28000</v>
+      </c>
+      <c r="H23" s="2">
+        <v>12</v>
+      </c>
+      <c r="I23" s="2">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J23" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K23" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="L23" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="M23" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="3:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="2">
+        <v>1</v>
+      </c>
+      <c r="F24" s="5"/>
+      <c r="G24" s="2">
+        <v>28000</v>
+      </c>
+      <c r="H24" s="2">
+        <v>13</v>
+      </c>
+      <c r="I24" s="2">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J24" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K24" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="L24" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="M24" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="3:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" s="2">
+        <v>2</v>
+      </c>
+      <c r="F25" s="5"/>
+      <c r="G25" s="2">
+        <v>28000</v>
+      </c>
+      <c r="H25" s="2">
+        <v>22</v>
+      </c>
+      <c r="I25" s="2">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J25" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K25" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="L25" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="M25" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="3:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" s="2">
+        <v>2</v>
+      </c>
+      <c r="F26" s="5"/>
+      <c r="G26" s="2">
+        <v>28000</v>
+      </c>
+      <c r="H26" s="2">
+        <v>23</v>
+      </c>
+      <c r="I26" s="2">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J26" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K26" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="L26" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="M26" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="3:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" s="2">
+        <v>2</v>
+      </c>
+      <c r="F27" s="5"/>
+      <c r="G27" s="2">
+        <v>28000</v>
+      </c>
+      <c r="H27" s="2">
+        <v>24</v>
+      </c>
+      <c r="I27" s="2">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J27" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K27" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="L27" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="M27" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="3:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="3">
+        <v>2</v>
+      </c>
+      <c r="F28" s="15"/>
+      <c r="G28" s="3">
+        <v>28000</v>
+      </c>
+      <c r="H28" s="3">
+        <v>25</v>
+      </c>
+      <c r="I28" s="3">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J28" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="K28" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="L28" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="M28" s="22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>28000</v>
+      </c>
+      <c r="H29">
         <v>14</v>
       </c>
-      <c r="D14" t="s">
+      <c r="I29">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J29" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="K29" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="L29" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="M29" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="3:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>28000</v>
+      </c>
+      <c r="H30">
+        <v>15</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J30" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="K30" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="L30" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="M30" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>28000</v>
+      </c>
+      <c r="H31">
         <v>16</v>
       </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="H14" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="H15" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="H16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="H17" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="H18" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="H19" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="H20" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="H21" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" t="s">
-        <v>21</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="H22" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" t="s">
-        <v>25</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-      <c r="H23" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" t="s">
-        <v>28</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-      <c r="H24" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" t="s">
-        <v>36</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-      <c r="H25" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27" t="s">
-        <v>22</v>
-      </c>
-      <c r="E27">
-        <v>2</v>
-      </c>
-      <c r="H27" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" t="s">
-        <v>26</v>
-      </c>
-      <c r="E28">
-        <v>2</v>
-      </c>
-      <c r="H28" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29" t="s">
-        <v>27</v>
-      </c>
-      <c r="E29">
-        <v>2</v>
-      </c>
-      <c r="H29" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
-        <v>14</v>
-      </c>
-      <c r="D30" t="s">
-        <v>23</v>
-      </c>
-      <c r="E30">
-        <v>2</v>
-      </c>
-      <c r="H30" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I31">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J31" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="K31" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="L31" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="M31" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>30</v>
+        <v>92</v>
       </c>
       <c r="E32">
         <v>1</v>
       </c>
-      <c r="H32" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="33" spans="3:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G32">
+        <v>28000</v>
+      </c>
+      <c r="H32">
+        <v>17</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J32" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="K32" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="L32" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="M32" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D33" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E33">
         <v>1</v>
       </c>
-      <c r="H33" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G33">
+        <v>28000</v>
+      </c>
+      <c r="H33">
+        <v>18</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J33" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="K33" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="L33" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="M33" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D34" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E34">
         <v>1</v>
       </c>
-      <c r="H34" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="35" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G34">
+        <v>28000</v>
+      </c>
+      <c r="H34">
+        <v>19</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J34" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="K34" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="L34" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="M34" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D35" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E35">
         <v>1</v>
       </c>
-      <c r="H35" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>32</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="G35">
+        <v>28000</v>
+      </c>
+      <c r="H35">
+        <v>20</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J35" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="K35" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="L35" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="M35" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="3:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C36" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E36" s="3">
+        <v>1</v>
+      </c>
+      <c r="F36" s="15"/>
+      <c r="G36" s="3">
+        <v>28000</v>
+      </c>
+      <c r="H36" s="3">
+        <v>21</v>
+      </c>
+      <c r="I36" s="3">
+        <f t="shared" si="0"/>
+        <v>28256</v>
+      </c>
+      <c r="J36" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="K36" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="L36" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="M36" s="22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
         <v>37</v>
       </c>
-      <c r="E36">
-        <v>1</v>
-      </c>
-      <c r="H36" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="37" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
-        <v>32</v>
-      </c>
       <c r="D37" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="E37">
-        <v>1</v>
-      </c>
-      <c r="H37" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="38" spans="3:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="J37" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K37" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="L37" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="M37" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="38" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D38" t="s">
+        <v>100</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+      <c r="J38" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K38" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="L38" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="M38" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="39" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39" t="s">
+        <v>101</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+      <c r="J39" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K39" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="L39" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="M39" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>37</v>
+      </c>
+      <c r="D40" t="s">
+        <v>106</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="J40" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K40" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="L40" s="21"/>
+      <c r="M40" s="21"/>
+    </row>
+    <row r="41" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>37</v>
+      </c>
+      <c r="D41" t="s">
+        <v>105</v>
+      </c>
+      <c r="E41">
+        <v>2</v>
+      </c>
+      <c r="J41" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K41" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="L41" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="M41" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="3:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C42" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E42" s="2">
+        <v>2</v>
+      </c>
+      <c r="F42" s="5"/>
+      <c r="J42" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K42" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="L42" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="M42" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>40</v>
+      </c>
+      <c r="D43" t="s">
         <v>38</v>
-      </c>
-      <c r="E38">
-        <v>1</v>
-      </c>
-      <c r="H38" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="39" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
-        <v>32</v>
-      </c>
-      <c r="D39" t="s">
-        <v>29</v>
-      </c>
-      <c r="E39">
-        <v>1</v>
-      </c>
-      <c r="H39" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="43" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
-        <v>39</v>
-      </c>
-      <c r="D43" t="s">
-        <v>46</v>
       </c>
       <c r="E43">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="F43" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J43" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K43" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="L43" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="M43" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44" spans="3:13" ht="26.25" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D44" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E44">
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="F44" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="J44" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K44" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="L44" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="M44" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="D45" t="s">
+        <v>48</v>
       </c>
       <c r="E45">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="F45" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="J45" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K45" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="L45" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="M45" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="D46" t="s">
+        <v>102</v>
       </c>
       <c r="E46">
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C47" t="s">
+      <c r="F46" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="J46" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K46" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="L46" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="M46" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="47" spans="3:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C47" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E47" s="3">
+        <v>2</v>
+      </c>
+      <c r="F47" s="15"/>
+      <c r="J47" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K47" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="L47" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="M47" s="22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="48" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C48" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="D48" t="s">
+        <v>112</v>
+      </c>
+      <c r="E48" s="16">
+        <v>2</v>
+      </c>
+      <c r="J48" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="K48" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="L48" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="M48" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="49" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C49" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="D49" t="s">
+        <v>113</v>
+      </c>
+      <c r="E49" s="16">
+        <v>2</v>
+      </c>
+      <c r="J49" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="K49" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="L49" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="M49" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="50" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C50" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="D50" t="s">
+        <v>114</v>
+      </c>
+      <c r="E50" s="16">
+        <v>2</v>
+      </c>
+      <c r="J50" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="K50" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="L50" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="M50" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="51" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C51" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="D51" t="s">
+        <v>115</v>
+      </c>
+      <c r="E51" s="16">
+        <v>2</v>
+      </c>
+      <c r="J51" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="K51" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="L51" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="M51" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="52" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C52" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="D52" t="s">
+        <v>116</v>
+      </c>
+      <c r="E52" s="16">
+        <v>2</v>
+      </c>
+      <c r="J52" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="K52" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="L52" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="M52" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="53" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C53" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="D53" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="16">
+        <v>2</v>
+      </c>
+      <c r="J53" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="K53" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="L53" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="M53" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="54" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C54" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="D54" t="s">
+        <v>117</v>
+      </c>
+      <c r="E54" s="16">
+        <v>2</v>
+      </c>
+      <c r="J54" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="K54" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="L54" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="M54" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="55" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C55" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="D55" t="s">
+        <v>118</v>
+      </c>
+      <c r="E55" s="16">
+        <v>2</v>
+      </c>
+      <c r="J55" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="K55" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="L55" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="M55" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="56" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C56" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="D56" t="s">
+        <v>119</v>
+      </c>
+      <c r="E56" s="16">
+        <v>2</v>
+      </c>
+      <c r="J56" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="K56" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="L56" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="M56" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="57" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C57" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="D57" t="s">
+        <v>120</v>
+      </c>
+      <c r="E57" s="16">
+        <v>2</v>
+      </c>
+      <c r="J57" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="K57" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="L57" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="M57" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="58" spans="3:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C58" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E58" s="3">
+        <v>2</v>
+      </c>
+      <c r="F58" s="15"/>
+      <c r="J58" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="K58" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="L58" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="M58" s="22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="59" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C59" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="D59" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="16">
+        <v>2</v>
+      </c>
+      <c r="J59" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="K59" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="L59" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="M59" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="60" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C60" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="D60" t="s">
+        <v>9</v>
+      </c>
+      <c r="E60" s="16">
+        <v>2</v>
+      </c>
+      <c r="J60" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="K60" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="L60" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="M60" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="61" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C61" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="D61" t="s">
+        <v>10</v>
+      </c>
+      <c r="E61" s="16">
+        <v>2</v>
+      </c>
+      <c r="J61" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="K61" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="L61" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="M61" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="62" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C62" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="D62" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" s="16">
+        <v>2</v>
+      </c>
+      <c r="J62" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="K62" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="L62" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="M62" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="63" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C63" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="D63" t="s">
+        <v>12</v>
+      </c>
+      <c r="E63" s="16">
+        <v>2</v>
+      </c>
+      <c r="J63" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="K63" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="L63" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="M63" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="64" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C64" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="D64" t="s">
+        <v>96</v>
+      </c>
+      <c r="E64" s="16">
+        <v>2</v>
+      </c>
+      <c r="J64" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="K64" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="L64" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="M64" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="65" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C65" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="D65" t="s">
+        <v>23</v>
+      </c>
+      <c r="E65" s="16">
+        <v>2</v>
+      </c>
+      <c r="J65" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="K65" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="L65" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="M65" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="66" spans="3:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C66" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="D66" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E47">
+      <c r="E66" s="17">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C48" t="s">
-        <v>39</v>
-      </c>
-      <c r="E48">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C49" t="s">
-        <v>39</v>
-      </c>
-      <c r="E49">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
-        <v>39</v>
-      </c>
-      <c r="E50">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C54" t="s">
-        <v>42</v>
-      </c>
-      <c r="D54" t="s">
-        <v>40</v>
-      </c>
-      <c r="E54">
-        <v>2</v>
-      </c>
-      <c r="F54" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="H54" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="55" spans="3:8" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="C55" t="s">
-        <v>42</v>
-      </c>
-      <c r="D55" t="s">
-        <v>48</v>
-      </c>
-      <c r="E55">
-        <v>2</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H55" t="s">
-        <v>80</v>
+      <c r="F66" s="15"/>
+      <c r="J66" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="K66" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="L66" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="M66" s="22" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:F37"/>
+  <autoFilter ref="A2:M36"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -2434,13 +3903,13 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.25" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.125" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.625" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.375" style="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.875" style="10" bestFit="1" customWidth="1"/>
@@ -2453,7 +3922,7 @@
   <sheetData>
     <row r="1" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -2467,42 +3936,42 @@
         <v>3</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>7</v>
+        <v>93</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G3" s="10">
         <v>25</v>
@@ -2511,27 +3980,27 @@
         <v>102</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>7</v>
+        <v>93</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G4" s="10">
         <v>25</v>
@@ -2540,27 +4009,27 @@
         <v>102</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>7</v>
+        <v>93</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G5" s="10">
         <v>25</v>
@@ -2569,27 +4038,27 @@
         <v>102</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>7</v>
+        <v>93</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G6" s="10">
         <v>5</v>
@@ -2598,27 +4067,27 @@
         <v>20</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>7</v>
+        <v>93</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G7" s="10">
         <v>5</v>
@@ -2627,27 +4096,27 @@
         <v>20</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>7</v>
+        <v>93</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G8" s="10">
         <v>3</v>
@@ -2656,36 +4125,36 @@
         <v>7</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>57</v>
-      </c>
       <c r="E9" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="G9" s="10">
-        <v>13</v>
-      </c>
-      <c r="H9" s="10">
-        <v>170</v>
+        <v>90</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>90</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2705,10 +4174,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2717,35 +4186,39 @@
     <col min="2" max="2" width="5.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5" customWidth="1"/>
-    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>41342</v>
       </c>
@@ -2753,71 +4226,92 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="F3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>122</v>
+      </c>
       <c r="B4" s="13">
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="F4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>84</v>
+      </c>
       <c r="B5" s="13">
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>84</v>
+      </c>
       <c r="B6" s="13">
         <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>84</v>
+      </c>
       <c r="B7" s="13">
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>84</v>
+      </c>
       <c r="B8" s="13">
         <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="13"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="13"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="13"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="13"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="13"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="13"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="13"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" s="13"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
@@ -2855,7 +4349,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -3021,16 +4515,16 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>876300</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>85725</xdr:colOff>
+                    <xdr:colOff>0</xdr:colOff>
                     <xdr:row>6</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3109,16 +4603,16 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>866775</xdr:colOff>
                     <xdr:row>7</xdr:row>
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>4</xdr:col>
-                    <xdr:colOff>85725</xdr:colOff>
-                    <xdr:row>8</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>714375</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>190500</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>

</xml_diff>